<commit_message>
24/04/2020 import TestData from Excel File V1.0
</commit_message>
<xml_diff>
--- a/mobileId/TestData/TestData_getToken.xlsx
+++ b/mobileId/TestData/TestData_getToken.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MobileId\202003_Sprint#9 CCR001-CCR003\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Strezzo06-PC\PycharmProjects\CWNTEST\mobileId\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7486DC80-1E22-496C-9D25-2061ECB4A088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4FA91B-629E-4ECA-830D-C7E0FDB57821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="405" windowWidth="14220" windowHeight="15195" xr2:uid="{95D47359-B412-490E-BDEF-E3A5DABEB81C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95D47359-B412-490E-BDEF-E3A5DABEB81C}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData_getToken" sheetId="1" r:id="rId1"/>
@@ -64,13 +64,13 @@
     <t>00333356868iulgiljkjjykykukuk4k3</t>
   </si>
   <si>
-    <t>${username}</t>
-  </si>
-  <si>
-    <t>${password}</t>
-  </si>
-  <si>
-    <t>${TC_No}</t>
+    <t>TC_No</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,13 +472,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2020/06/02 - Input Data from Excel and write PASS/FAILED to Excel getToken V1.0
</commit_message>
<xml_diff>
--- a/mobileId/TestData/TestData_getToken.xlsx
+++ b/mobileId/TestData/TestData_getToken.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Strezzo06-PC\PycharmProjects\CWNTEST\mobileId\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panruethai.e\PycharmProjects\CWNTEST\mobileId\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4FA91B-629E-4ECA-830D-C7E0FDB57821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95D47359-B412-490E-BDEF-E3A5DABEB81C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="TestData_getToken" sheetId="1" r:id="rId1"/>
     <sheet name="Data List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Chaincode API_getToken_Issuer_001</t>
   </si>
@@ -67,16 +66,25 @@
     <t>TC_No</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
+    <t>200</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Status Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -114,32 +122,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -455,11 +451,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3848A9A-40CC-463F-A2DC-3DBDAB0D2AF0}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,22 +463,26 @@
     <col min="1" max="1" width="32" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -491,9 +491,12 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -502,9 +505,12 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -513,9 +519,12 @@
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -524,9 +533,12 @@
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -534,6 +546,9 @@
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -543,7 +558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A852467-93DD-417A-9F80-67BB7700D87B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>